<commit_message>
La till koordinater i excelfilen
</commit_message>
<xml_diff>
--- a/Project/data/Studentuppgift fiktiv planering.xlsx
+++ b/Project/data/Studentuppgift fiktiv planering.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Samordnare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\GitHub\Projekt\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E571407-CE37-47AB-898A-3A218E4FBD9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCAF697-EEB6-4E26-9521-6D1BD7CA4B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="1070" activeTab="1" xr2:uid="{DF7C8647-7540-4BF1-8D10-1CB10261A2CC}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21150" activeTab="2" xr2:uid="{DF7C8647-7540-4BF1-8D10-1CB10261A2CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Individer, brukare" sheetId="1" r:id="rId1"/>
     <sheet name="Medarbetare" sheetId="2" r:id="rId2"/>
+    <sheet name="Koordinater" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="205">
   <si>
     <t>Behöver läkemedel</t>
   </si>
@@ -629,13 +630,25 @@
   </si>
   <si>
     <t>25 schemarader, varav det alltid är 9 st på förmiddagen och 5 st på kvällen</t>
+  </si>
+  <si>
+    <t>North:</t>
+  </si>
+  <si>
+    <t>South:</t>
+  </si>
+  <si>
+    <t>West:</t>
+  </si>
+  <si>
+    <t>East:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,6 +663,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -701,35 +720,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,9 +761,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -789,7 +801,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -895,7 +907,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1037,7 +1049,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1045,37 +1057,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B758A53-16F2-4A2D-AD1B-C01B6DCB7923}">
-  <dimension ref="A1:V78"/>
+  <dimension ref="A1:U78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="3"/>
-    <col min="2" max="2" width="8.81640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="29.08984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.7265625" style="8"/>
-    <col min="9" max="9" width="10.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.08984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.7265625" style="8"/>
-    <col min="15" max="15" width="14.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7265625" style="8"/>
-    <col min="17" max="17" width="12.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.7265625" style="8"/>
-    <col min="19" max="19" width="13.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.54296875" style="3" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="8"/>
+    <col min="1" max="1" width="8.7109375" style="3"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:22" s="1" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1136,56 +1143,56 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="K3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="4">
         <v>30</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="5">
-        <v>10</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="5">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="5" t="s">
+      <c r="M3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="4">
+        <v>10</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="R3" s="4">
@@ -1194,2226 +1201,2181 @@
       <c r="S3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="T3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="5">
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="4">
         <v>30</v>
       </c>
-      <c r="M4" s="5">
-        <v>10</v>
-      </c>
-      <c r="N4" s="5">
+      <c r="M4" s="4">
+        <v>10</v>
+      </c>
+      <c r="N4" s="4">
         <v>15</v>
       </c>
-      <c r="O4" s="5">
-        <v>10</v>
-      </c>
-      <c r="P4" s="5">
+      <c r="O4" s="4">
+        <v>10</v>
+      </c>
+      <c r="P4" s="4">
         <v>15</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4" s="4">
         <v>15</v>
       </c>
-      <c r="R4" s="5">
+      <c r="R4" s="4">
         <v>20</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="5">
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="4">
         <v>15</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" s="5">
+      <c r="O5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="4">
         <v>15</v>
       </c>
-      <c r="Q5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="T5" s="6" t="s">
+      <c r="Q5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="5">
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="4">
         <v>15</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="S6" s="5" t="s">
+      <c r="M6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="T6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="5">
+      <c r="E7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="4">
         <v>20</v>
       </c>
-      <c r="M7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7" s="5">
+      <c r="M7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="4">
         <v>15</v>
       </c>
-      <c r="O7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P7" s="5">
+      <c r="O7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" s="4">
         <v>15</v>
       </c>
-      <c r="Q7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="S7" s="5" t="s">
+      <c r="Q7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="T7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="5" t="s">
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="P8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="4">
         <v>15</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="S8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="T8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="T8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="5" t="s">
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="R9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="S9" s="5" t="s">
+      <c r="J9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="T9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="T9" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="4">
         <v>20</v>
       </c>
-      <c r="M10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="R10" s="8">
+      <c r="M10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10">
         <v>20</v>
       </c>
-      <c r="S10" s="5"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="S10" s="4"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="6" t="s">
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="S12" s="5"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="S12" s="4"/>
+      <c r="T12" s="5"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="5">
-        <v>10</v>
-      </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="4">
+        <v>10</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4">
         <v>15</v>
       </c>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="5"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="5" t="s">
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5" t="s">
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="Q14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="Q14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="5">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="4">
         <v>25</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="4">
         <v>15</v>
       </c>
-      <c r="O15" s="5" t="s">
+      <c r="O15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P15" s="5">
+      <c r="P15" s="4">
         <v>20</v>
       </c>
-      <c r="Q15" s="5" t="s">
+      <c r="Q15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="8">
+      <c r="R15">
         <v>15</v>
       </c>
-      <c r="S15" s="5"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="7" t="s">
+      <c r="S15" s="4"/>
+      <c r="T15" s="5"/>
+      <c r="U15" t="s">
         <v>41</v>
       </c>
-      <c r="V15" s="7"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="5">
-        <v>10</v>
-      </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5">
-        <v>10</v>
-      </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5">
-        <v>10</v>
-      </c>
-      <c r="R16" s="8">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="4">
+        <v>10</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4">
+        <v>10</v>
+      </c>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4">
+        <v>10</v>
+      </c>
+      <c r="R16">
         <v>5</v>
       </c>
-      <c r="S16" s="5" t="s">
+      <c r="S16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="T16" s="6"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="5">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="4">
         <v>15</v>
       </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5">
-        <v>10</v>
-      </c>
-      <c r="O17" s="5">
+      <c r="M17" s="4"/>
+      <c r="N17" s="4">
+        <v>10</v>
+      </c>
+      <c r="O17" s="4">
         <v>5</v>
       </c>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5">
-        <v>10</v>
-      </c>
-      <c r="R17" s="5">
-        <v>10</v>
-      </c>
-      <c r="S17" s="5" t="s">
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4">
+        <v>10</v>
+      </c>
+      <c r="R17" s="4">
+        <v>10</v>
+      </c>
+      <c r="S17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="T17" s="6"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="5">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="4">
         <v>15</v>
       </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5">
+      <c r="M18" s="4"/>
+      <c r="N18" s="4">
         <v>15</v>
       </c>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5">
-        <v>10</v>
-      </c>
-      <c r="Q18" s="5">
+      <c r="O18" s="4"/>
+      <c r="P18" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="4">
         <v>7</v>
       </c>
-      <c r="S18" s="5" t="s">
+      <c r="S18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="T18" s="6"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="5">
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="4">
         <v>20</v>
       </c>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="5" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5">
+      <c r="M20" s="4"/>
+      <c r="N20" s="4">
         <v>20</v>
       </c>
-      <c r="O20" s="5">
+      <c r="O20" s="4">
         <v>20</v>
       </c>
-      <c r="P20" s="5">
+      <c r="P20" s="4">
         <v>20</v>
       </c>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5">
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4">
         <v>20</v>
       </c>
-      <c r="S20" s="7"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="7" t="s">
+      <c r="U20" t="s">
         <v>41</v>
       </c>
-      <c r="V20" s="7"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="5">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="4">
         <v>15</v>
       </c>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5">
+      <c r="M21" s="4"/>
+      <c r="N21" s="4">
         <v>15</v>
       </c>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5">
+      <c r="O21" s="4"/>
+      <c r="P21" s="4">
         <v>15</v>
       </c>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="8">
+      <c r="Q21" s="4"/>
+      <c r="R21">
         <v>15</v>
       </c>
-      <c r="S21" s="7"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="5">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="4">
         <v>5</v>
       </c>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5">
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4">
         <v>5</v>
       </c>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="8">
-        <v>10</v>
-      </c>
-      <c r="S22" s="7"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="7" t="s">
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22">
+        <v>10</v>
+      </c>
+      <c r="U22" t="s">
         <v>49</v>
       </c>
-      <c r="V22" s="7"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" s="5">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="4">
         <v>5</v>
       </c>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5">
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4">
         <v>5</v>
       </c>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="8">
-        <v>10</v>
-      </c>
-      <c r="U23" s="8" t="s">
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23">
+        <v>10</v>
+      </c>
+      <c r="U23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="5">
-        <v>10</v>
-      </c>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="8">
-        <v>10</v>
-      </c>
-      <c r="S24" s="8" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="4">
+        <v>10</v>
+      </c>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24">
+        <v>10</v>
+      </c>
+      <c r="S24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="5">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="4">
         <v>7</v>
       </c>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="8">
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5" t="s">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="5">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="4">
         <v>40</v>
       </c>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5">
+      <c r="M26" s="4"/>
+      <c r="N26" s="4">
         <v>15</v>
       </c>
-      <c r="O26" s="5">
+      <c r="O26" s="4">
         <v>20</v>
       </c>
-      <c r="P26" s="5">
+      <c r="P26" s="4">
         <v>15</v>
       </c>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5">
-        <v>10</v>
-      </c>
-      <c r="S26" s="8" t="s">
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4">
+        <v>10</v>
+      </c>
+      <c r="S26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N27" s="8" t="s">
+      <c r="N27" t="s">
         <v>36</v>
       </c>
       <c r="T27" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="J28" t="s">
         <v>25</v>
       </c>
-      <c r="L28" s="5">
-        <v>10</v>
-      </c>
-      <c r="R28" s="8">
-        <v>10</v>
-      </c>
-      <c r="S28" s="8" t="s">
+      <c r="L28" s="4">
+        <v>10</v>
+      </c>
+      <c r="R28">
+        <v>10</v>
+      </c>
+      <c r="S28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" t="s">
         <v>19</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L29" s="5">
-        <v>10</v>
-      </c>
-      <c r="N29" s="8">
+      <c r="L29" s="4">
+        <v>10</v>
+      </c>
+      <c r="N29">
         <v>5</v>
       </c>
-      <c r="R29" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="R29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="5">
-        <v>10</v>
-      </c>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="4">
+        <v>10</v>
+      </c>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4">
         <v>15</v>
       </c>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5">
-        <v>10</v>
-      </c>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5" t="s">
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4">
+        <v>10</v>
+      </c>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="T30" s="6"/>
-      <c r="U30" s="8" t="s">
+      <c r="T30" s="5"/>
+      <c r="U30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>122</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="5">
-        <v>10</v>
-      </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="4">
+        <v>10</v>
+      </c>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4">
         <v>15</v>
       </c>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5" t="s">
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="T31" s="6"/>
-      <c r="U31" s="8" t="s">
+      <c r="T31" s="5"/>
+      <c r="U31" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="5">
-        <v>10</v>
-      </c>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="6"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="4">
+        <v>10</v>
+      </c>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="5"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="5">
-        <v>10</v>
-      </c>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="6"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="4">
+        <v>10</v>
+      </c>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="5"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B34" s="4"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5" t="s">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="6"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="5"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4">
         <v>30</v>
       </c>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="6"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="5"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5" t="s">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="6" t="s">
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B37" s="4"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="6" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B38" s="4"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="5">
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="4">
         <v>20</v>
       </c>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5">
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4">
         <v>20</v>
       </c>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="6"/>
-      <c r="U38" s="8" t="s">
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="5"/>
+      <c r="U38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>130</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="5">
-        <v>10</v>
-      </c>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="6" t="s">
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="4">
+        <v>10</v>
+      </c>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="U39" s="8" t="s">
+      <c r="U39" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="5">
-        <v>10</v>
-      </c>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="6" t="s">
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="4">
+        <v>10</v>
+      </c>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="U40" s="8" t="s">
+      <c r="U40" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="5">
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="4">
         <v>5</v>
       </c>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5">
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4">
         <v>5</v>
       </c>
-      <c r="S41" s="5"/>
-      <c r="T41" s="6"/>
-      <c r="U41" s="8" t="s">
+      <c r="S41" s="4"/>
+      <c r="T41" s="5"/>
+      <c r="U41" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>133</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5" t="s">
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K42" s="6"/>
-      <c r="L42" s="5" t="s">
+      <c r="K42" s="5"/>
+      <c r="L42" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="M42" s="5">
-        <v>10</v>
-      </c>
-      <c r="N42" s="5" t="s">
+      <c r="M42" s="4">
+        <v>10</v>
+      </c>
+      <c r="N42" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5" t="s">
+      <c r="O42" s="4"/>
+      <c r="P42" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5" t="s">
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="S42" s="5" t="s">
+      <c r="S42" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="T42" s="6"/>
-      <c r="U42" s="8" t="s">
+      <c r="T42" s="5"/>
+      <c r="U42" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="5">
-        <v>10</v>
-      </c>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5">
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="4">
+        <v>10</v>
+      </c>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4">
         <v>15</v>
       </c>
-      <c r="O43" s="5">
-        <v>10</v>
-      </c>
-      <c r="P43" s="5">
-        <v>10</v>
-      </c>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5">
-        <v>10</v>
-      </c>
-      <c r="S43" s="5"/>
-      <c r="T43" s="6"/>
-      <c r="U43" s="8" t="s">
+      <c r="O43" s="4">
+        <v>10</v>
+      </c>
+      <c r="P43" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4">
+        <v>10</v>
+      </c>
+      <c r="S43" s="4"/>
+      <c r="T43" s="5"/>
+      <c r="U43" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5" t="s">
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="6" t="s">
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="6" t="s">
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B46" s="4"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5">
-        <v>10</v>
-      </c>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4">
+        <v>10</v>
+      </c>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="T46" s="6"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="T46" s="5"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>138</v>
       </c>
       <c r="B47" s="4"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5" t="s">
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="6" t="s">
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>139</v>
       </c>
       <c r="B48" s="4"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5" t="s">
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="5">
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="4">
         <v>15</v>
       </c>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="5"/>
-      <c r="R48" s="5"/>
-      <c r="S48" s="5"/>
-      <c r="T48" s="6"/>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="5"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B49" s="4"/>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="5">
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="4">
         <v>5</v>
       </c>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-      <c r="R49" s="5">
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4">
         <v>5</v>
       </c>
-      <c r="S49" s="5"/>
-      <c r="T49" s="6"/>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="S49" s="4"/>
+      <c r="T49" s="5"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B50" s="4"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5" t="s">
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-      <c r="R50" s="5"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="6"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="5"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B51" s="4"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
-      <c r="R51" s="5"/>
-      <c r="S51" s="5"/>
-      <c r="T51" s="6" t="s">
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B52" s="4"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="5">
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="4">
         <v>15</v>
       </c>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="5">
-        <v>10</v>
-      </c>
-      <c r="S52" s="5"/>
-      <c r="T52" s="6" t="s">
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4">
+        <v>10</v>
+      </c>
+      <c r="S52" s="4"/>
+      <c r="T52" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B53" s="4"/>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="5">
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="4">
         <v>20</v>
       </c>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5">
+      <c r="M53" s="4"/>
+      <c r="N53" s="4">
         <v>15</v>
       </c>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5">
+      <c r="O53" s="4"/>
+      <c r="P53" s="4">
         <v>15</v>
       </c>
-      <c r="Q53" s="5"/>
-      <c r="R53" s="5">
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4">
         <v>15</v>
       </c>
-      <c r="S53" s="5" t="s">
+      <c r="S53" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T53" s="6" t="s">
+      <c r="T53" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B54" s="4"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5" t="s">
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="P54" s="5"/>
-      <c r="Q54" s="5" t="s">
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="R54" s="5"/>
-      <c r="S54" s="5"/>
-      <c r="T54" s="6"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="5"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="5">
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="4">
         <v>15</v>
       </c>
-      <c r="M55" s="5">
-        <v>10</v>
-      </c>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5">
-        <v>10</v>
-      </c>
-      <c r="Q55" s="5">
-        <v>10</v>
-      </c>
-      <c r="R55" s="5"/>
-      <c r="S55" s="5" t="s">
+      <c r="M55" s="4">
+        <v>10</v>
+      </c>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>10</v>
+      </c>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="T55" s="6"/>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="T55" s="5"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" t="s">
         <v>80</v>
       </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="5">
-        <v>10</v>
-      </c>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5">
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="4">
+        <v>10</v>
+      </c>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4">
         <v>15</v>
       </c>
-      <c r="O56" s="5"/>
-      <c r="P56" s="5">
+      <c r="O56" s="4"/>
+      <c r="P56" s="4">
         <v>15</v>
       </c>
-      <c r="Q56" s="5">
-        <v>10</v>
-      </c>
-      <c r="R56" s="5"/>
-      <c r="S56" s="5" t="s">
+      <c r="Q56" s="4">
+        <v>10</v>
+      </c>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="T56" s="6"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="T56" s="5"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="N57" s="5"/>
-      <c r="O57" s="5"/>
-      <c r="P57" s="5"/>
-      <c r="Q57" s="5"/>
-      <c r="R57" s="5"/>
-      <c r="S57" s="5"/>
-      <c r="T57" s="6" t="s">
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" t="s">
         <v>24</v>
       </c>
-      <c r="L58" s="5">
+      <c r="L58" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B59" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M59" s="8">
+      <c r="B59" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59">
         <v>20</v>
       </c>
-      <c r="P59" s="8">
+      <c r="P59">
         <v>20</v>
       </c>
-      <c r="Q59" s="8">
+      <c r="Q59">
         <v>20</v>
       </c>
-      <c r="U59" s="8" t="s">
+      <c r="U59" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="J60" s="8" t="s">
+      <c r="J60" t="s">
         <v>83</v>
       </c>
-      <c r="S60" s="8" t="s">
+      <c r="S60" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="L61" s="8">
+      <c r="L61">
         <v>20</v>
       </c>
-      <c r="N61" s="8">
+      <c r="N61">
         <v>15</v>
       </c>
-      <c r="O61" s="8">
-        <v>10</v>
-      </c>
-      <c r="R61" s="8">
+      <c r="O61">
+        <v>10</v>
+      </c>
+      <c r="R61">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B62" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M62" s="8">
-        <v>10</v>
-      </c>
-      <c r="Q62" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>19</v>
+      </c>
+      <c r="M62">
+        <v>10</v>
+      </c>
+      <c r="Q62">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B63" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J63" s="8" t="s">
+      <c r="B63" t="s">
+        <v>19</v>
+      </c>
+      <c r="J63" t="s">
         <v>83</v>
       </c>
-      <c r="M63" s="8">
-        <v>10</v>
-      </c>
-      <c r="Q63" s="8">
-        <v>10</v>
-      </c>
-      <c r="S63" s="8" t="s">
+      <c r="M63">
+        <v>10</v>
+      </c>
+      <c r="Q63">
+        <v>10</v>
+      </c>
+      <c r="S63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D64" t="s">
         <v>24</v>
       </c>
-      <c r="L64" s="8" t="s">
+      <c r="L64" t="s">
         <v>69</v>
       </c>
-      <c r="M64" s="8">
-        <v>10</v>
-      </c>
-      <c r="N64" s="8">
+      <c r="M64">
+        <v>10</v>
+      </c>
+      <c r="N64">
         <v>15</v>
       </c>
-      <c r="O64" s="8">
+      <c r="O64">
         <v>15</v>
       </c>
-      <c r="P64" s="8">
+      <c r="P64">
         <v>15</v>
       </c>
-      <c r="Q64" s="8">
+      <c r="Q64">
         <v>30</v>
       </c>
-      <c r="S64" s="8" t="s">
+      <c r="S64" t="s">
         <v>54</v>
       </c>
       <c r="T64" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" t="s">
         <v>51</v>
       </c>
-      <c r="L65" s="8" t="s">
+      <c r="L65" t="s">
         <v>85</v>
       </c>
-      <c r="R65" s="8">
+      <c r="R65">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="S66" s="8" t="s">
+      <c r="S66" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" t="s">
         <v>24</v>
       </c>
-      <c r="L67" s="8">
-        <v>10</v>
-      </c>
-      <c r="P67" s="8">
-        <v>10</v>
-      </c>
-      <c r="Q67" s="8">
+      <c r="L67">
+        <v>10</v>
+      </c>
+      <c r="P67">
+        <v>10</v>
+      </c>
+      <c r="Q67">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="M68" s="8" t="s">
+      <c r="M68" t="s">
         <v>36</v>
       </c>
-      <c r="R68" s="8" t="s">
+      <c r="R68" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" t="s">
         <v>87</v>
       </c>
-      <c r="L69" s="8">
-        <v>10</v>
-      </c>
-      <c r="N69" s="8">
-        <v>10</v>
-      </c>
-      <c r="P69" s="8">
-        <v>10</v>
-      </c>
-      <c r="Q69" s="8">
-        <v>10</v>
-      </c>
-      <c r="S69" s="8" t="s">
+      <c r="L69">
+        <v>10</v>
+      </c>
+      <c r="N69">
+        <v>10</v>
+      </c>
+      <c r="P69">
+        <v>10</v>
+      </c>
+      <c r="Q69">
+        <v>10</v>
+      </c>
+      <c r="S69" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="L70" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="L70">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="J71" s="8" t="s">
+      <c r="J71" t="s">
         <v>25</v>
       </c>
-      <c r="L71" s="8">
+      <c r="L71">
         <v>5</v>
       </c>
-      <c r="O71" s="8">
+      <c r="O71">
         <v>5</v>
       </c>
-      <c r="P71" s="8">
+      <c r="P71">
         <v>5</v>
       </c>
-      <c r="Q71" s="8">
+      <c r="Q71">
         <v>5</v>
       </c>
-      <c r="S71" s="8" t="s">
+      <c r="S71" t="s">
         <v>88</v>
       </c>
       <c r="T71" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="M72" s="8">
-        <v>10</v>
-      </c>
-      <c r="R72" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B74" s="14" t="s">
+      <c r="M72">
+        <v>10</v>
+      </c>
+      <c r="R72">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B74" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B75" s="12" t="s">
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B75" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B76" s="13" t="s">
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B76" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B78" s="10" t="s">
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3427,29 +3389,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1E7D1B-68D6-4AE2-80BA-48299DF7C7ED}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" customWidth="1"/>
-    <col min="10" max="10" width="7.6328125" customWidth="1"/>
-    <col min="11" max="11" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>198</v>
       </c>
@@ -3481,7 +3443,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -3516,7 +3478,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -3551,7 +3513,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>166</v>
       </c>
@@ -3586,7 +3548,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>167</v>
       </c>
@@ -3621,7 +3583,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>168</v>
       </c>
@@ -3656,7 +3618,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>169</v>
       </c>
@@ -3691,7 +3653,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>170</v>
       </c>
@@ -3726,7 +3688,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>171</v>
       </c>
@@ -3761,7 +3723,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -3796,7 +3758,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>173</v>
       </c>
@@ -3831,7 +3793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>174</v>
       </c>
@@ -3866,7 +3828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>175</v>
       </c>
@@ -3901,7 +3863,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -3936,7 +3898,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>177</v>
       </c>
@@ -3971,7 +3933,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>178</v>
       </c>
@@ -4006,7 +3968,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -4041,7 +4003,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>180</v>
       </c>
@@ -4076,7 +4038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -4111,7 +4073,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -4146,7 +4108,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -4181,7 +4143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>184</v>
       </c>
@@ -4216,7 +4178,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>185</v>
       </c>
@@ -4251,7 +4213,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>186</v>
       </c>
@@ -4286,7 +4248,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>187</v>
       </c>
@@ -4321,7 +4283,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>188</v>
       </c>
@@ -4354,6 +4316,57 @@
       </c>
       <c r="K28" t="s">
         <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41546C5E-97C1-4332-B37F-C0710C216F81}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="9">
+        <v>64.840199999999996</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="9">
+        <v>64.646199999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="9">
+        <v>21.3169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="9">
+        <v>20.848600000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>